<commit_message>
test correctif json 279a1e38837d7491e7fae206564a0dbcd92ca45a
</commit_message>
<xml_diff>
--- a/ig/sd-add-extension-eclaire-description-summary/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/sd-add-extension-eclaire-description-summary/StructureDefinition-eclaire-researchstudy.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-01-23T09:22:43+00:00</t>
+    <t>2024-01-23T10:11:47+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -541,6 +541,22 @@
     <t>Extension créée dans le cadre du projet API ECLAIRE afin de pouvoir renseigner le(s) promoteur(s) secondaire(s)</t>
   </si>
   <si>
+    <t>ResearchStudy.extension:eclaire-description-summary-r5</t>
+  </si>
+  <si>
+    <t>eclaire-description-summary-r5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/5.0/StructureDefinition/extension-ResearchStudy.descriptionSummary}
+</t>
+  </si>
+  <si>
+    <t>Texte bref décrivant l'essai / Brief text explaining the study.</t>
+  </si>
+  <si>
+    <t>Cette extension implemente l'élément descriptionSummary de R5. elle permet l'ajout d'un texte bref décrivant l'essai</t>
+  </si>
+  <si>
     <t>ResearchStudy.extension:eclaire-label-r5</t>
   </si>
   <si>
@@ -555,22 +571,6 @@
   </si>
   <si>
     <t>Cette extension implemente l'élément label de R5. elle permet l'ajout de plusieurs titres pour l'essai</t>
-  </si>
-  <si>
-    <t>ResearchStudy.extension:eclaire-description-summary-r5</t>
-  </si>
-  <si>
-    <t>eclaire-description-summary-r5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {http://hl7.org/fhir/5.0/StructureDefinition/extension-ResearchStudy.descriptionSummary}
-</t>
-  </si>
-  <si>
-    <t>Texte bref décrivant l'essai / Brief text explaining the study.</t>
-  </si>
-  <si>
-    <t>Cette extension implemente l'élément descriptionSummary de R5. elle permet l'ajout d'un texte bref décrivant l'essai.</t>
   </si>
   <si>
     <t>ResearchStudy.modifierExtension</t>
@@ -3784,7 +3784,7 @@
         <v>78</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H14" t="s" s="2">
         <v>91</v>
@@ -3874,7 +3874,7 @@
         <v>80</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="AN14" t="s" s="2">
         <v>80</v>
@@ -3901,7 +3901,7 @@
         <v>78</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>91</v>
@@ -3991,7 +3991,7 @@
         <v>80</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="AN15" t="s" s="2">
         <v>80</v>

</xml_diff>